<commit_message>
minor changes and new training trials
</commit_message>
<xml_diff>
--- a/src/omniroute_operation/src/single_T_maze/Training_Trials _testing4.xlsx
+++ b/src/omniroute_operation/src/single_T_maze/Training_Trials _testing4.xlsx
@@ -102,6 +102,7 @@
       <color rgb="FF000000"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="11"/>
@@ -113,16 +114,15 @@
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
-      <name val="Arial"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
-      <name val="Calibri"/>
+      <name val="Arial"/>
       <family val="2"/>
-      <charset val="1"/>
     </font>
   </fonts>
   <fills count="2">
@@ -215,11 +215,11 @@
   </sheetPr>
   <dimension ref="A1:G109"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A34" colorId="64" zoomScale="250" zoomScaleNormal="250" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G67" activeCellId="0" sqref="G67"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A10" colorId="64" zoomScale="250" zoomScaleNormal="250" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="I32" activeCellId="0" sqref="I32"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.12109375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.13671875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="true" outlineLevel="0" max="5" min="5" style="0" width="11.71"/>
   </cols>
@@ -259,18 +259,18 @@
       </c>
       <c r="E2" s="1" t="n">
         <f aca="true">RAND()</f>
-        <v>0.700041483223732</v>
+        <v>0.130414509001467</v>
       </c>
       <c r="F2" s="4" t="n">
         <f aca="true">RAND()</f>
-        <v>0.756013490344006</v>
+        <v>0.557292916006217</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="5" t="s">
-        <v>6</v>
-      </c>
-      <c r="B3" s="5" t="s">
+      <c r="A3" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B3" s="2" t="s">
         <v>7</v>
       </c>
       <c r="C3" s="3" t="s">
@@ -281,21 +281,21 @@
       </c>
       <c r="E3" s="1" t="n">
         <f aca="true">RAND()</f>
-        <v>0.818427303376948</v>
+        <v>0.858072327679966</v>
       </c>
       <c r="F3" s="4" t="n">
         <f aca="true">RAND()</f>
-        <v>0.947444268331411</v>
+        <v>0.821859172118679</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="5" t="s">
-        <v>6</v>
-      </c>
-      <c r="B4" s="5" t="s">
-        <v>7</v>
-      </c>
-      <c r="C4" s="6" t="s">
+      <c r="A4" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C4" s="5" t="s">
         <v>8</v>
       </c>
       <c r="D4" s="1" t="s">
@@ -303,18 +303,18 @@
       </c>
       <c r="E4" s="1" t="n">
         <f aca="true">RAND()</f>
-        <v>0.194751665731869</v>
+        <v>0.947680655627702</v>
       </c>
       <c r="F4" s="4" t="n">
         <f aca="true">RAND()</f>
-        <v>0.031361506982374</v>
+        <v>0.849452084171307</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="5" t="s">
-        <v>7</v>
-      </c>
-      <c r="B5" s="5" t="s">
+      <c r="A5" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B5" s="2" t="s">
         <v>6</v>
       </c>
       <c r="C5" s="3" t="s">
@@ -325,21 +325,21 @@
       </c>
       <c r="E5" s="1" t="n">
         <f aca="true">RAND()</f>
-        <v>0.983334497835601</v>
+        <v>0.677243285599695</v>
       </c>
       <c r="F5" s="4" t="n">
         <f aca="true">RAND()</f>
-        <v>0.680156810212988</v>
+        <v>0.142201441910988</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="5" t="s">
-        <v>7</v>
-      </c>
-      <c r="B6" s="5" t="s">
-        <v>6</v>
-      </c>
-      <c r="C6" s="6" t="s">
+      <c r="A6" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C6" s="5" t="s">
         <v>8</v>
       </c>
       <c r="D6" s="1" t="s">
@@ -347,18 +347,18 @@
       </c>
       <c r="E6" s="1" t="n">
         <f aca="true">RAND()</f>
-        <v>0.536265333792816</v>
+        <v>0.933510445098754</v>
       </c>
       <c r="F6" s="4" t="n">
         <f aca="true">RAND()</f>
-        <v>0.372786865960179</v>
+        <v>0.107638917234766</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="5" t="s">
-        <v>7</v>
-      </c>
-      <c r="B7" s="5" t="s">
+      <c r="A7" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B7" s="2" t="s">
         <v>6</v>
       </c>
       <c r="C7" s="3" t="s">
@@ -369,18 +369,18 @@
       </c>
       <c r="E7" s="1" t="n">
         <f aca="true">RAND()</f>
-        <v>0.240270145574803</v>
+        <v>0.858342983571697</v>
       </c>
       <c r="F7" s="4" t="n">
         <f aca="true">RAND()</f>
-        <v>0.21504923592679</v>
+        <v>0.182781466623008</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="5" t="s">
-        <v>7</v>
-      </c>
-      <c r="B8" s="5" t="s">
+      <c r="A8" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B8" s="2" t="s">
         <v>6</v>
       </c>
       <c r="C8" s="3" t="s">
@@ -391,18 +391,18 @@
       </c>
       <c r="E8" s="1" t="n">
         <f aca="true">RAND()</f>
-        <v>0.269565465502349</v>
+        <v>0.699747956089845</v>
       </c>
       <c r="F8" s="4" t="n">
         <f aca="true">RAND()</f>
-        <v>0.681376916657308</v>
+        <v>0.721141958313153</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="5" t="s">
-        <v>6</v>
-      </c>
-      <c r="B9" s="5" t="s">
+      <c r="A9" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B9" s="2" t="s">
         <v>7</v>
       </c>
       <c r="C9" s="3" t="s">
@@ -413,18 +413,18 @@
       </c>
       <c r="E9" s="1" t="n">
         <f aca="true">RAND()</f>
-        <v>0.663032173181299</v>
+        <v>0.412820771208752</v>
       </c>
       <c r="F9" s="4" t="n">
         <f aca="true">RAND()</f>
-        <v>0.664691610708569</v>
+        <v>0.306197814133643</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="5" t="s">
-        <v>7</v>
-      </c>
-      <c r="B10" s="5" t="s">
+      <c r="A10" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B10" s="2" t="s">
         <v>6</v>
       </c>
       <c r="C10" s="3" t="s">
@@ -435,18 +435,18 @@
       </c>
       <c r="E10" s="1" t="n">
         <f aca="true">RAND()</f>
-        <v>0.0405972383654824</v>
+        <v>0.170720183686509</v>
       </c>
       <c r="F10" s="4" t="n">
         <f aca="true">RAND()</f>
-        <v>0.980382644521474</v>
+        <v>0.743328050060121</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="5" t="s">
-        <v>6</v>
-      </c>
-      <c r="B11" s="5" t="s">
+      <c r="A11" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B11" s="2" t="s">
         <v>7</v>
       </c>
       <c r="C11" s="3" t="s">
@@ -457,18 +457,18 @@
       </c>
       <c r="E11" s="1" t="n">
         <f aca="true">RAND()</f>
-        <v>0.375367330458136</v>
+        <v>0.73807150111061</v>
       </c>
       <c r="F11" s="4" t="n">
         <f aca="true">RAND()</f>
-        <v>0.354309344983994</v>
+        <v>0.424782758631647</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="5" t="s">
-        <v>7</v>
-      </c>
-      <c r="B12" s="5" t="s">
+      <c r="A12" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B12" s="2" t="s">
         <v>6</v>
       </c>
       <c r="C12" s="3" t="s">
@@ -479,24 +479,24 @@
       </c>
       <c r="E12" s="1" t="n">
         <f aca="true">RAND()</f>
-        <v>0.537073884387347</v>
+        <v>0.0786894915823644</v>
       </c>
       <c r="F12" s="4" t="n">
         <f aca="true">RAND()</f>
-        <v>0.30703132457851</v>
+        <v>0.746479640648669</v>
       </c>
       <c r="G12" s="0" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="5" t="s">
-        <v>7</v>
-      </c>
-      <c r="B13" s="5" t="s">
-        <v>6</v>
-      </c>
-      <c r="C13" s="6" t="s">
+      <c r="A13" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B13" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C13" s="5" t="s">
         <v>8</v>
       </c>
       <c r="D13" s="1" t="s">
@@ -504,11 +504,11 @@
       </c>
       <c r="E13" s="1" t="n">
         <f aca="true">RAND()</f>
-        <v>0.0170490287236629</v>
+        <v>0.885892089650997</v>
       </c>
       <c r="F13" s="4" t="n">
         <f aca="true">RAND()</f>
-        <v>0.093692818572112</v>
+        <v>0.516846232853057</v>
       </c>
       <c r="G13" s="0" t="s">
         <v>10</v>
@@ -521,7 +521,7 @@
       <c r="B14" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="C14" s="6" t="s">
+      <c r="C14" s="5" t="s">
         <v>8</v>
       </c>
       <c r="D14" s="1" t="s">
@@ -529,24 +529,24 @@
       </c>
       <c r="E14" s="1" t="n">
         <f aca="true">RAND()</f>
-        <v>0.0467115622963932</v>
+        <v>0.413872433353575</v>
       </c>
       <c r="F14" s="4" t="n">
         <f aca="true">RAND()</f>
-        <v>0.48828157026474</v>
+        <v>0.144927969860287</v>
       </c>
       <c r="G14" s="0" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="5" t="s">
-        <v>7</v>
-      </c>
-      <c r="B15" s="5" t="s">
-        <v>6</v>
-      </c>
-      <c r="C15" s="6" t="s">
+      <c r="A15" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B15" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C15" s="5" t="s">
         <v>8</v>
       </c>
       <c r="D15" s="1" t="s">
@@ -554,24 +554,24 @@
       </c>
       <c r="E15" s="1" t="n">
         <f aca="true">RAND()</f>
-        <v>0.466424572148332</v>
+        <v>0.43220941856484</v>
       </c>
       <c r="F15" s="4" t="n">
         <f aca="true">RAND()</f>
-        <v>0.92813013304765</v>
+        <v>0.537646065645024</v>
       </c>
       <c r="G15" s="0" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="5" t="s">
-        <v>6</v>
-      </c>
-      <c r="B16" s="5" t="s">
-        <v>7</v>
-      </c>
-      <c r="C16" s="6" t="s">
+      <c r="A16" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B16" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C16" s="5" t="s">
         <v>8</v>
       </c>
       <c r="D16" s="1" t="s">
@@ -579,24 +579,24 @@
       </c>
       <c r="E16" s="1" t="n">
         <f aca="true">RAND()</f>
-        <v>0.245155403410731</v>
+        <v>0.876868754760905</v>
       </c>
       <c r="F16" s="4" t="n">
         <f aca="true">RAND()</f>
-        <v>0.55407425409447</v>
+        <v>0.729719374894168</v>
       </c>
       <c r="G16" s="0" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="5" t="s">
-        <v>6</v>
-      </c>
-      <c r="B17" s="5" t="s">
-        <v>7</v>
-      </c>
-      <c r="C17" s="6" t="s">
+      <c r="A17" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B17" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C17" s="5" t="s">
         <v>8</v>
       </c>
       <c r="D17" s="1" t="s">
@@ -604,24 +604,24 @@
       </c>
       <c r="E17" s="1" t="n">
         <f aca="true">RAND()</f>
-        <v>0.62275689208046</v>
+        <v>0.674749916999289</v>
       </c>
       <c r="F17" s="4" t="n">
         <f aca="true">RAND()</f>
-        <v>0.800705894619597</v>
+        <v>0.29139534741473</v>
       </c>
       <c r="G17" s="0" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="5" t="s">
-        <v>6</v>
-      </c>
-      <c r="B18" s="5" t="s">
-        <v>7</v>
-      </c>
-      <c r="C18" s="6" t="s">
+      <c r="A18" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B18" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C18" s="5" t="s">
         <v>8</v>
       </c>
       <c r="D18" s="1" t="s">
@@ -629,24 +629,24 @@
       </c>
       <c r="E18" s="1" t="n">
         <f aca="true">RAND()</f>
-        <v>0.737287662824097</v>
+        <v>0.872238026448905</v>
       </c>
       <c r="F18" s="4" t="n">
         <f aca="true">RAND()</f>
-        <v>0.827563707737282</v>
+        <v>0.153670128996562</v>
       </c>
       <c r="G18" s="0" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A19" s="5" t="s">
-        <v>6</v>
-      </c>
-      <c r="B19" s="5" t="s">
-        <v>7</v>
-      </c>
-      <c r="C19" s="6" t="s">
+      <c r="A19" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B19" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C19" s="5" t="s">
         <v>8</v>
       </c>
       <c r="D19" s="1" t="s">
@@ -654,24 +654,24 @@
       </c>
       <c r="E19" s="1" t="n">
         <f aca="true">RAND()</f>
-        <v>0.746422331049244</v>
+        <v>0.15550262457403</v>
       </c>
       <c r="F19" s="4" t="n">
         <f aca="true">RAND()</f>
-        <v>0.039980736389891</v>
+        <v>0.507193400117411</v>
       </c>
       <c r="G19" s="0" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A20" s="5" t="s">
-        <v>7</v>
-      </c>
-      <c r="B20" s="5" t="s">
-        <v>6</v>
-      </c>
-      <c r="C20" s="6" t="s">
+      <c r="A20" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B20" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C20" s="5" t="s">
         <v>8</v>
       </c>
       <c r="D20" s="1" t="s">
@@ -679,24 +679,24 @@
       </c>
       <c r="E20" s="1" t="n">
         <f aca="true">RAND()</f>
-        <v>0.860608210343922</v>
+        <v>0.572852447991213</v>
       </c>
       <c r="F20" s="4" t="n">
         <f aca="true">RAND()</f>
-        <v>0.635799832406719</v>
+        <v>0.95056517851097</v>
       </c>
       <c r="G20" s="0" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A21" s="5" t="s">
-        <v>6</v>
-      </c>
-      <c r="B21" s="5" t="s">
-        <v>7</v>
-      </c>
-      <c r="C21" s="6" t="s">
+      <c r="A21" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B21" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C21" s="5" t="s">
         <v>8</v>
       </c>
       <c r="D21" s="1" t="s">
@@ -704,24 +704,24 @@
       </c>
       <c r="E21" s="1" t="n">
         <f aca="true">RAND()</f>
-        <v>0.708264409230287</v>
+        <v>0.607017045800267</v>
       </c>
       <c r="F21" s="4" t="n">
         <f aca="true">RAND()</f>
-        <v>0.686363694707732</v>
+        <v>0.22915832397244</v>
       </c>
       <c r="G21" s="0" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A22" s="5" t="s">
-        <v>7</v>
-      </c>
-      <c r="B22" s="5" t="s">
-        <v>6</v>
-      </c>
-      <c r="C22" s="6" t="s">
+      <c r="A22" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B22" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C22" s="5" t="s">
         <v>8</v>
       </c>
       <c r="D22" s="1" t="s">
@@ -729,24 +729,24 @@
       </c>
       <c r="E22" s="1" t="n">
         <f aca="true">RAND()</f>
-        <v>0.850703943852095</v>
+        <v>0.661812505037233</v>
       </c>
       <c r="F22" s="0" t="n">
         <f aca="true">RAND()</f>
-        <v>0.326155654090174</v>
+        <v>0.781867749270291</v>
       </c>
       <c r="G22" s="0" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A23" s="5" t="s">
-        <v>6</v>
-      </c>
-      <c r="B23" s="5" t="s">
-        <v>7</v>
-      </c>
-      <c r="C23" s="6" t="s">
+      <c r="A23" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B23" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C23" s="5" t="s">
         <v>8</v>
       </c>
       <c r="D23" s="1" t="s">
@@ -754,24 +754,24 @@
       </c>
       <c r="E23" s="1" t="n">
         <f aca="true">RAND()</f>
-        <v>0.930750515588292</v>
+        <v>0.304428002010308</v>
       </c>
       <c r="F23" s="0" t="n">
         <f aca="true">RAND()</f>
-        <v>0.450829122752427</v>
+        <v>0.34306934295004</v>
       </c>
       <c r="G23" s="0" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A24" s="5" t="s">
-        <v>7</v>
-      </c>
-      <c r="B24" s="5" t="s">
-        <v>6</v>
-      </c>
-      <c r="C24" s="6" t="s">
+      <c r="A24" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B24" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C24" s="5" t="s">
         <v>8</v>
       </c>
       <c r="D24" s="1" t="s">
@@ -779,24 +779,24 @@
       </c>
       <c r="E24" s="1" t="n">
         <f aca="true">RAND()</f>
-        <v>0.554621851184384</v>
+        <v>0.977395111286957</v>
       </c>
       <c r="F24" s="0" t="n">
         <f aca="true">RAND()</f>
-        <v>0.522471459583395</v>
+        <v>0.00681045473732927</v>
       </c>
       <c r="G24" s="0" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A25" s="5" t="s">
-        <v>7</v>
-      </c>
-      <c r="B25" s="5" t="s">
-        <v>6</v>
-      </c>
-      <c r="C25" s="6" t="s">
+      <c r="A25" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B25" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C25" s="5" t="s">
         <v>8</v>
       </c>
       <c r="D25" s="1" t="s">
@@ -804,24 +804,24 @@
       </c>
       <c r="E25" s="1" t="n">
         <f aca="true">RAND()</f>
-        <v>0.993303465798543</v>
+        <v>0.189820648781044</v>
       </c>
       <c r="F25" s="0" t="n">
         <f aca="true">RAND()</f>
-        <v>0.535153958827296</v>
+        <v>0.367760865315169</v>
       </c>
       <c r="G25" s="0" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A26" s="5" t="s">
-        <v>6</v>
-      </c>
-      <c r="B26" s="5" t="s">
-        <v>7</v>
-      </c>
-      <c r="C26" s="6" t="s">
+      <c r="A26" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B26" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C26" s="5" t="s">
         <v>8</v>
       </c>
       <c r="D26" s="1" t="s">
@@ -829,24 +829,24 @@
       </c>
       <c r="E26" s="1" t="n">
         <f aca="true">RAND()</f>
-        <v>0.630697268710942</v>
+        <v>0.76832890521938</v>
       </c>
       <c r="F26" s="0" t="n">
         <f aca="true">RAND()</f>
-        <v>0.216496351637571</v>
+        <v>0.19422948745107</v>
       </c>
       <c r="G26" s="0" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A27" s="5" t="s">
-        <v>7</v>
-      </c>
-      <c r="B27" s="5" t="s">
-        <v>6</v>
-      </c>
-      <c r="C27" s="6" t="s">
+      <c r="A27" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B27" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C27" s="5" t="s">
         <v>12</v>
       </c>
       <c r="D27" s="1" t="s">
@@ -854,24 +854,24 @@
       </c>
       <c r="E27" s="1" t="n">
         <f aca="true">RAND()</f>
-        <v>0.745495338720369</v>
+        <v>0.365948512215637</v>
       </c>
       <c r="F27" s="0" t="n">
         <f aca="true">RAND()</f>
-        <v>0.766813631680681</v>
+        <v>0.54568792786292</v>
       </c>
       <c r="G27" s="0" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A28" s="5" t="s">
-        <v>7</v>
-      </c>
-      <c r="B28" s="5" t="s">
-        <v>6</v>
-      </c>
-      <c r="C28" s="6" t="s">
+      <c r="A28" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B28" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C28" s="5" t="s">
         <v>12</v>
       </c>
       <c r="D28" s="1" t="s">
@@ -879,24 +879,24 @@
       </c>
       <c r="E28" s="1" t="n">
         <f aca="true">RAND()</f>
-        <v>0.611401574615314</v>
+        <v>0.274482061749475</v>
       </c>
       <c r="F28" s="0" t="n">
         <f aca="true">RAND()</f>
-        <v>0.0851541020698552</v>
+        <v>0.223890567029579</v>
       </c>
       <c r="G28" s="0" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A29" s="5" t="s">
-        <v>7</v>
-      </c>
-      <c r="B29" s="5" t="s">
-        <v>6</v>
-      </c>
-      <c r="C29" s="6" t="s">
+      <c r="A29" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B29" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C29" s="5" t="s">
         <v>12</v>
       </c>
       <c r="D29" s="1" t="s">
@@ -904,24 +904,24 @@
       </c>
       <c r="E29" s="1" t="n">
         <f aca="true">RAND()</f>
-        <v>0.404934665181788</v>
+        <v>0.720339746421759</v>
       </c>
       <c r="F29" s="0" t="n">
         <f aca="true">RAND()</f>
-        <v>0.665771656673756</v>
+        <v>0.159609495168484</v>
       </c>
       <c r="G29" s="0" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A30" s="5" t="s">
-        <v>6</v>
-      </c>
-      <c r="B30" s="5" t="s">
-        <v>7</v>
-      </c>
-      <c r="C30" s="6" t="s">
+      <c r="A30" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B30" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C30" s="5" t="s">
         <v>12</v>
       </c>
       <c r="D30" s="1" t="s">
@@ -929,24 +929,24 @@
       </c>
       <c r="E30" s="1" t="n">
         <f aca="true">RAND()</f>
-        <v>0.348316839598557</v>
+        <v>0.223845217620051</v>
       </c>
       <c r="F30" s="0" t="n">
         <f aca="true">RAND()</f>
-        <v>0.199168937268411</v>
+        <v>0.628067986790935</v>
       </c>
       <c r="G30" s="0" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A31" s="5" t="s">
-        <v>6</v>
-      </c>
-      <c r="B31" s="5" t="s">
-        <v>7</v>
-      </c>
-      <c r="C31" s="6" t="s">
+      <c r="A31" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B31" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C31" s="5" t="s">
         <v>12</v>
       </c>
       <c r="D31" s="1" t="s">
@@ -954,24 +954,24 @@
       </c>
       <c r="E31" s="1" t="n">
         <f aca="true">RAND()</f>
-        <v>0.420358325972626</v>
+        <v>0.0815105621902264</v>
       </c>
       <c r="F31" s="0" t="n">
         <f aca="true">RAND()</f>
-        <v>0.185100928241624</v>
+        <v>0.144097429573024</v>
       </c>
       <c r="G31" s="0" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A32" s="5" t="s">
-        <v>7</v>
-      </c>
-      <c r="B32" s="5" t="s">
-        <v>6</v>
-      </c>
-      <c r="C32" s="6" t="s">
+      <c r="A32" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B32" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C32" s="5" t="s">
         <v>12</v>
       </c>
       <c r="D32" s="1" t="s">
@@ -979,24 +979,24 @@
       </c>
       <c r="E32" s="1" t="n">
         <f aca="true">RAND()</f>
-        <v>0.842228033574094</v>
+        <v>0.998928844930602</v>
       </c>
       <c r="F32" s="0" t="n">
         <f aca="true">RAND()</f>
-        <v>0.464056174731064</v>
+        <v>0.142895597562851</v>
       </c>
       <c r="G32" s="0" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A33" s="5" t="s">
-        <v>6</v>
-      </c>
-      <c r="B33" s="5" t="s">
-        <v>7</v>
-      </c>
-      <c r="C33" s="6" t="s">
+      <c r="A33" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="B33" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="C33" s="5" t="s">
         <v>12</v>
       </c>
       <c r="D33" s="1" t="s">
@@ -1004,24 +1004,24 @@
       </c>
       <c r="E33" s="1" t="n">
         <f aca="true">RAND()</f>
-        <v>0.377523037867055</v>
+        <v>0.647270044373275</v>
       </c>
       <c r="F33" s="0" t="n">
         <f aca="true">RAND()</f>
-        <v>0.476796460888872</v>
+        <v>0.514326933035572</v>
       </c>
       <c r="G33" s="0" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A34" s="5" t="s">
-        <v>7</v>
-      </c>
-      <c r="B34" s="5" t="s">
-        <v>6</v>
-      </c>
-      <c r="C34" s="6" t="s">
+      <c r="A34" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B34" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C34" s="5" t="s">
         <v>12</v>
       </c>
       <c r="D34" s="1" t="s">
@@ -1029,24 +1029,24 @@
       </c>
       <c r="E34" s="1" t="n">
         <f aca="true">RAND()</f>
-        <v>0.585938526750547</v>
+        <v>0.211480469735495</v>
       </c>
       <c r="F34" s="0" t="n">
         <f aca="true">RAND()</f>
-        <v>0.15870627158784</v>
+        <v>0.724117207019224</v>
       </c>
       <c r="G34" s="0" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A35" s="5" t="s">
-        <v>6</v>
-      </c>
-      <c r="B35" s="5" t="s">
-        <v>7</v>
-      </c>
-      <c r="C35" s="6" t="s">
+      <c r="A35" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B35" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C35" s="5" t="s">
         <v>12</v>
       </c>
       <c r="D35" s="1" t="s">
@@ -1054,24 +1054,24 @@
       </c>
       <c r="E35" s="1" t="n">
         <f aca="true">RAND()</f>
-        <v>0.907583455472936</v>
+        <v>0.627111839676822</v>
       </c>
       <c r="F35" s="0" t="n">
         <f aca="true">RAND()</f>
-        <v>0.347112299335679</v>
+        <v>0.0941846787190433</v>
       </c>
       <c r="G35" s="0" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A36" s="5" t="s">
-        <v>7</v>
-      </c>
-      <c r="B36" s="5" t="s">
-        <v>6</v>
-      </c>
-      <c r="C36" s="6" t="s">
+      <c r="A36" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B36" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C36" s="5" t="s">
         <v>12</v>
       </c>
       <c r="D36" s="1" t="s">
@@ -1079,24 +1079,24 @@
       </c>
       <c r="E36" s="1" t="n">
         <f aca="true">RAND()</f>
-        <v>0.884729300668416</v>
+        <v>0.97193700785838</v>
       </c>
       <c r="F36" s="0" t="n">
         <f aca="true">RAND()</f>
-        <v>0.953608234150384</v>
+        <v>0.306756485868035</v>
       </c>
       <c r="G36" s="0" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A37" s="5" t="s">
-        <v>6</v>
-      </c>
-      <c r="B37" s="5" t="s">
-        <v>7</v>
-      </c>
-      <c r="C37" s="6" t="s">
+      <c r="A37" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B37" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C37" s="5" t="s">
         <v>12</v>
       </c>
       <c r="D37" s="1" t="s">
@@ -1104,24 +1104,24 @@
       </c>
       <c r="E37" s="1" t="n">
         <f aca="true">RAND()</f>
-        <v>0.0408282193309433</v>
+        <v>0.410631575257119</v>
       </c>
       <c r="F37" s="0" t="n">
         <f aca="true">RAND()</f>
-        <v>0.718608068449455</v>
+        <v>0.384596024012711</v>
       </c>
       <c r="G37" s="0" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A38" s="5" t="s">
-        <v>6</v>
-      </c>
-      <c r="B38" s="5" t="s">
-        <v>7</v>
-      </c>
-      <c r="C38" s="6" t="s">
+      <c r="A38" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B38" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C38" s="5" t="s">
         <v>12</v>
       </c>
       <c r="D38" s="1" t="s">
@@ -1129,24 +1129,24 @@
       </c>
       <c r="E38" s="1" t="n">
         <f aca="true">RAND()</f>
-        <v>0.843234102930174</v>
+        <v>0.135444302635051</v>
       </c>
       <c r="F38" s="0" t="n">
         <f aca="true">RAND()</f>
-        <v>0.196492437709548</v>
+        <v>0.681639725117321</v>
       </c>
       <c r="G38" s="0" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A39" s="5" t="s">
-        <v>6</v>
-      </c>
-      <c r="B39" s="5" t="s">
-        <v>7</v>
-      </c>
-      <c r="C39" s="6" t="s">
+      <c r="A39" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B39" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C39" s="5" t="s">
         <v>12</v>
       </c>
       <c r="D39" s="1" t="s">
@@ -1154,24 +1154,24 @@
       </c>
       <c r="E39" s="1" t="n">
         <f aca="true">RAND()</f>
-        <v>0.268005647653342</v>
+        <v>0.581178077901493</v>
       </c>
       <c r="F39" s="0" t="n">
         <f aca="true">RAND()</f>
-        <v>0.808136360939787</v>
+        <v>0.115990428625541</v>
       </c>
       <c r="G39" s="0" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A40" s="5" t="s">
-        <v>7</v>
-      </c>
-      <c r="B40" s="5" t="s">
-        <v>6</v>
-      </c>
-      <c r="C40" s="6" t="s">
+      <c r="A40" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B40" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C40" s="5" t="s">
         <v>12</v>
       </c>
       <c r="D40" s="1" t="s">
@@ -1179,24 +1179,24 @@
       </c>
       <c r="E40" s="1" t="n">
         <f aca="true">RAND()</f>
-        <v>0.819055544944916</v>
+        <v>0.79059909327794</v>
       </c>
       <c r="F40" s="0" t="n">
         <f aca="true">RAND()</f>
-        <v>0.142917176287971</v>
+        <v>0.0384309103839942</v>
       </c>
       <c r="G40" s="0" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="41" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A41" s="5" t="s">
-        <v>6</v>
-      </c>
-      <c r="B41" s="5" t="s">
-        <v>7</v>
-      </c>
-      <c r="C41" s="6" t="s">
+      <c r="A41" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B41" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C41" s="5" t="s">
         <v>12</v>
       </c>
       <c r="D41" s="1" t="s">
@@ -1204,24 +1204,24 @@
       </c>
       <c r="E41" s="1" t="n">
         <f aca="true">RAND()</f>
-        <v>0.245695944482126</v>
+        <v>0.82792794608623</v>
       </c>
       <c r="F41" s="0" t="n">
         <f aca="true">RAND()</f>
-        <v>0.0541847560815434</v>
+        <v>0.727218978179593</v>
       </c>
       <c r="G41" s="0" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="42" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A42" s="5" t="s">
-        <v>7</v>
-      </c>
-      <c r="B42" s="5" t="s">
-        <v>6</v>
-      </c>
-      <c r="C42" s="6" t="s">
+      <c r="A42" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B42" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C42" s="5" t="s">
         <v>12</v>
       </c>
       <c r="D42" s="1" t="s">
@@ -1229,24 +1229,24 @@
       </c>
       <c r="E42" s="1" t="n">
         <f aca="true">RAND()</f>
-        <v>0.679177518988469</v>
+        <v>0.827065692638758</v>
       </c>
       <c r="F42" s="0" t="n">
         <f aca="true">RAND()</f>
-        <v>0.623649020833829</v>
+        <v>0.933397713137652</v>
       </c>
       <c r="G42" s="0" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="43" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A43" s="5" t="s">
-        <v>7</v>
-      </c>
-      <c r="B43" s="5" t="s">
-        <v>6</v>
-      </c>
-      <c r="C43" s="6" t="s">
+      <c r="A43" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B43" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C43" s="5" t="s">
         <v>12</v>
       </c>
       <c r="D43" s="1" t="s">
@@ -1254,24 +1254,24 @@
       </c>
       <c r="E43" s="1" t="n">
         <f aca="true">RAND()</f>
-        <v>0.639487680410246</v>
+        <v>0.512899533233217</v>
       </c>
       <c r="F43" s="0" t="n">
         <f aca="true">RAND()</f>
-        <v>0.24160614915048</v>
+        <v>0.28612559035515</v>
       </c>
       <c r="G43" s="0" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="44" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A44" s="5" t="s">
-        <v>7</v>
-      </c>
-      <c r="B44" s="5" t="s">
-        <v>6</v>
-      </c>
-      <c r="C44" s="6" t="s">
+      <c r="A44" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B44" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C44" s="5" t="s">
         <v>12</v>
       </c>
       <c r="D44" s="1" t="s">
@@ -1279,24 +1279,24 @@
       </c>
       <c r="E44" s="1" t="n">
         <f aca="true">RAND()</f>
-        <v>0.717975924640478</v>
+        <v>0.0135855450347847</v>
       </c>
       <c r="F44" s="0" t="n">
         <f aca="true">RAND()</f>
-        <v>0.0161160132363617</v>
+        <v>0.348805039585844</v>
       </c>
       <c r="G44" s="0" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="45" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A45" s="5" t="s">
-        <v>7</v>
-      </c>
-      <c r="B45" s="5" t="s">
-        <v>6</v>
-      </c>
-      <c r="C45" s="6" t="s">
+      <c r="A45" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B45" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C45" s="5" t="s">
         <v>12</v>
       </c>
       <c r="D45" s="1" t="s">
@@ -1304,24 +1304,24 @@
       </c>
       <c r="E45" s="1" t="n">
         <f aca="true">RAND()</f>
-        <v>0.48410866522113</v>
+        <v>0.593020947369936</v>
       </c>
       <c r="F45" s="0" t="n">
         <f aca="true">RAND()</f>
-        <v>0.458636618528878</v>
+        <v>0.018307927028734</v>
       </c>
       <c r="G45" s="0" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="46" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A46" s="5" t="s">
-        <v>7</v>
-      </c>
-      <c r="B46" s="5" t="s">
-        <v>6</v>
-      </c>
-      <c r="C46" s="6" t="s">
+      <c r="A46" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B46" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C46" s="5" t="s">
         <v>12</v>
       </c>
       <c r="D46" s="1" t="s">
@@ -1329,24 +1329,24 @@
       </c>
       <c r="E46" s="1" t="n">
         <f aca="true">RAND()</f>
-        <v>0.050715758865979</v>
+        <v>0.803385384387806</v>
       </c>
       <c r="F46" s="0" t="n">
         <f aca="true">RAND()</f>
-        <v>0.411149151083483</v>
+        <v>0.0106818512512524</v>
       </c>
       <c r="G46" s="0" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="47" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A47" s="5" t="s">
-        <v>6</v>
-      </c>
-      <c r="B47" s="5" t="s">
-        <v>7</v>
-      </c>
-      <c r="C47" s="6" t="s">
+      <c r="A47" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B47" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C47" s="5" t="s">
         <v>12</v>
       </c>
       <c r="D47" s="1" t="s">
@@ -1354,24 +1354,24 @@
       </c>
       <c r="E47" s="1" t="n">
         <f aca="true">RAND()</f>
-        <v>0.31504578212586</v>
+        <v>0.120082759948207</v>
       </c>
       <c r="F47" s="0" t="n">
         <f aca="true">RAND()</f>
-        <v>0.640506775633144</v>
+        <v>0.667696889466302</v>
       </c>
       <c r="G47" s="0" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="48" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A48" s="5" t="s">
-        <v>6</v>
-      </c>
-      <c r="B48" s="5" t="s">
-        <v>7</v>
-      </c>
-      <c r="C48" s="6" t="s">
+      <c r="A48" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B48" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C48" s="5" t="s">
         <v>12</v>
       </c>
       <c r="D48" s="1" t="s">
@@ -1379,24 +1379,24 @@
       </c>
       <c r="E48" s="1" t="n">
         <f aca="true">RAND()</f>
-        <v>0.41826985983647</v>
+        <v>0.624857699994007</v>
       </c>
       <c r="F48" s="0" t="n">
         <f aca="true">RAND()</f>
-        <v>0.0976365552869024</v>
+        <v>0.295738053099945</v>
       </c>
       <c r="G48" s="0" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="49" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A49" s="5" t="s">
-        <v>6</v>
-      </c>
-      <c r="B49" s="5" t="s">
-        <v>7</v>
-      </c>
-      <c r="C49" s="6" t="s">
+      <c r="A49" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B49" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C49" s="5" t="s">
         <v>12</v>
       </c>
       <c r="D49" s="1" t="s">
@@ -1404,24 +1404,24 @@
       </c>
       <c r="E49" s="1" t="n">
         <f aca="true">RAND()</f>
-        <v>0.179845787348839</v>
+        <v>0.686453834329939</v>
       </c>
       <c r="F49" s="0" t="n">
         <f aca="true">RAND()</f>
-        <v>0.539930958228684</v>
+        <v>0.846190725807593</v>
       </c>
       <c r="G49" s="0" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="50" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A50" s="5" t="s">
-        <v>6</v>
-      </c>
-      <c r="B50" s="5" t="s">
-        <v>7</v>
-      </c>
-      <c r="C50" s="6" t="s">
+      <c r="A50" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B50" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C50" s="5" t="s">
         <v>12</v>
       </c>
       <c r="D50" s="1" t="s">
@@ -1429,24 +1429,24 @@
       </c>
       <c r="E50" s="1" t="n">
         <f aca="true">RAND()</f>
-        <v>0.693890816039141</v>
+        <v>0.682903991422083</v>
       </c>
       <c r="F50" s="0" t="n">
         <f aca="true">RAND()</f>
-        <v>0.921143503653727</v>
+        <v>0.416108281273153</v>
       </c>
       <c r="G50" s="0" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="51" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A51" s="5" t="s">
-        <v>7</v>
-      </c>
-      <c r="B51" s="5" t="s">
-        <v>6</v>
-      </c>
-      <c r="C51" s="6" t="s">
+      <c r="A51" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B51" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C51" s="5" t="s">
         <v>12</v>
       </c>
       <c r="D51" s="1" t="s">
@@ -1454,24 +1454,24 @@
       </c>
       <c r="E51" s="1" t="n">
         <f aca="true">RAND()</f>
-        <v>0.522294494139023</v>
+        <v>0.709191925144333</v>
       </c>
       <c r="F51" s="0" t="n">
         <f aca="true">RAND()</f>
-        <v>0.82228603934706</v>
+        <v>0.309670414656102</v>
       </c>
       <c r="G51" s="0" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="52" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A52" s="5" t="s">
-        <v>7</v>
-      </c>
-      <c r="B52" s="5" t="s">
-        <v>6</v>
-      </c>
-      <c r="C52" s="6" t="s">
+      <c r="A52" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B52" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C52" s="5" t="s">
         <v>12</v>
       </c>
       <c r="D52" s="1" t="s">
@@ -1479,24 +1479,24 @@
       </c>
       <c r="E52" s="1" t="n">
         <f aca="true">RAND()</f>
-        <v>0.619350523722439</v>
+        <v>0.609177146322934</v>
       </c>
       <c r="F52" s="0" t="n">
         <f aca="true">RAND()</f>
-        <v>0.417381078410396</v>
+        <v>0.644406976278056</v>
       </c>
       <c r="G52" s="0" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="53" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A53" s="5" t="s">
-        <v>7</v>
-      </c>
-      <c r="B53" s="5" t="s">
-        <v>6</v>
-      </c>
-      <c r="C53" s="6" t="s">
+      <c r="A53" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B53" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C53" s="5" t="s">
         <v>8</v>
       </c>
       <c r="D53" s="1" t="s">
@@ -1504,24 +1504,24 @@
       </c>
       <c r="E53" s="1" t="n">
         <f aca="true">RAND()</f>
-        <v>0.682707277995587</v>
+        <v>0.220409089634291</v>
       </c>
       <c r="F53" s="0" t="n">
         <f aca="true">RAND()</f>
-        <v>0.256438450788974</v>
+        <v>0.707281338758349</v>
       </c>
       <c r="G53" s="0" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="54" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A54" s="5" t="s">
-        <v>7</v>
-      </c>
-      <c r="B54" s="5" t="s">
-        <v>6</v>
-      </c>
-      <c r="C54" s="6" t="s">
+      <c r="A54" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B54" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C54" s="5" t="s">
         <v>8</v>
       </c>
       <c r="D54" s="1" t="s">
@@ -1529,24 +1529,24 @@
       </c>
       <c r="E54" s="1" t="n">
         <f aca="true">RAND()</f>
-        <v>0.0973905316289537</v>
+        <v>0.916215568798381</v>
       </c>
       <c r="F54" s="0" t="n">
         <f aca="true">RAND()</f>
-        <v>0.073588715396145</v>
+        <v>0.528699545084467</v>
       </c>
       <c r="G54" s="0" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="55" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A55" s="5" t="s">
-        <v>7</v>
-      </c>
-      <c r="B55" s="5" t="s">
-        <v>6</v>
-      </c>
-      <c r="C55" s="6" t="s">
+      <c r="A55" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B55" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C55" s="5" t="s">
         <v>12</v>
       </c>
       <c r="D55" s="1" t="s">
@@ -1554,24 +1554,24 @@
       </c>
       <c r="E55" s="1" t="n">
         <f aca="true">RAND()</f>
-        <v>0.841183754909459</v>
+        <v>0.0735028780973855</v>
       </c>
       <c r="F55" s="0" t="n">
         <f aca="true">RAND()</f>
-        <v>0.493826359118969</v>
+        <v>0.992341875042586</v>
       </c>
       <c r="G55" s="0" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="56" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A56" s="5" t="s">
-        <v>7</v>
-      </c>
-      <c r="B56" s="5" t="s">
-        <v>6</v>
-      </c>
-      <c r="C56" s="6" t="s">
+      <c r="A56" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B56" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C56" s="5" t="s">
         <v>8</v>
       </c>
       <c r="D56" s="1" t="s">
@@ -1579,24 +1579,24 @@
       </c>
       <c r="E56" s="1" t="n">
         <f aca="true">RAND()</f>
-        <v>0.461619600024708</v>
+        <v>0.458531167949859</v>
       </c>
       <c r="F56" s="0" t="n">
         <f aca="true">RAND()</f>
-        <v>0.755381215819233</v>
+        <v>0.87433279222654</v>
       </c>
       <c r="G56" s="0" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="57" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A57" s="5" t="s">
-        <v>6</v>
-      </c>
-      <c r="B57" s="5" t="s">
-        <v>7</v>
-      </c>
-      <c r="C57" s="6" t="s">
+      <c r="A57" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B57" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C57" s="5" t="s">
         <v>12</v>
       </c>
       <c r="D57" s="1" t="s">
@@ -1604,24 +1604,24 @@
       </c>
       <c r="E57" s="1" t="n">
         <f aca="true">RAND()</f>
-        <v>0.800021628413373</v>
+        <v>0.490281158507801</v>
       </c>
       <c r="F57" s="0" t="n">
         <f aca="true">RAND()</f>
-        <v>0.344161239959902</v>
+        <v>0.519055561335539</v>
       </c>
       <c r="G57" s="0" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="58" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A58" s="5" t="s">
-        <v>6</v>
-      </c>
-      <c r="B58" s="5" t="s">
-        <v>7</v>
-      </c>
-      <c r="C58" s="6" t="s">
+      <c r="A58" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B58" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C58" s="5" t="s">
         <v>8</v>
       </c>
       <c r="D58" s="1" t="s">
@@ -1629,24 +1629,24 @@
       </c>
       <c r="E58" s="1" t="n">
         <f aca="true">RAND()</f>
-        <v>0.184790986878781</v>
+        <v>0.743227997826092</v>
       </c>
       <c r="F58" s="0" t="n">
         <f aca="true">RAND()</f>
-        <v>0.528034909709195</v>
+        <v>0.187444169546398</v>
       </c>
       <c r="G58" s="0" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="59" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A59" s="5" t="s">
-        <v>6</v>
-      </c>
-      <c r="B59" s="5" t="s">
-        <v>7</v>
-      </c>
-      <c r="C59" s="6" t="s">
+      <c r="A59" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B59" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C59" s="5" t="s">
         <v>12</v>
       </c>
       <c r="D59" s="1" t="s">
@@ -1654,24 +1654,24 @@
       </c>
       <c r="E59" s="1" t="n">
         <f aca="true">RAND()</f>
-        <v>0.999542002386824</v>
+        <v>0.460620499708014</v>
       </c>
       <c r="F59" s="0" t="n">
         <f aca="true">RAND()</f>
-        <v>0.41746940159318</v>
+        <v>0.544056844942673</v>
       </c>
       <c r="G59" s="0" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="60" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A60" s="5" t="s">
-        <v>7</v>
-      </c>
-      <c r="B60" s="5" t="s">
-        <v>6</v>
-      </c>
-      <c r="C60" s="6" t="s">
+      <c r="A60" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B60" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C60" s="5" t="s">
         <v>12</v>
       </c>
       <c r="D60" s="1" t="s">
@@ -1679,24 +1679,24 @@
       </c>
       <c r="E60" s="1" t="n">
         <f aca="true">RAND()</f>
-        <v>0.153928660154695</v>
+        <v>0.113158889858619</v>
       </c>
       <c r="F60" s="0" t="n">
         <f aca="true">RAND()</f>
-        <v>0.783007318933999</v>
+        <v>0.913478018593701</v>
       </c>
       <c r="G60" s="0" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="61" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A61" s="5" t="s">
-        <v>6</v>
-      </c>
-      <c r="B61" s="5" t="s">
-        <v>7</v>
-      </c>
-      <c r="C61" s="6" t="s">
+      <c r="A61" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B61" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C61" s="5" t="s">
         <v>12</v>
       </c>
       <c r="D61" s="1" t="s">
@@ -1704,100 +1704,100 @@
       </c>
       <c r="E61" s="1" t="n">
         <f aca="true">RAND()</f>
-        <v>0.570323921167842</v>
+        <v>0.791859740683391</v>
       </c>
       <c r="F61" s="0" t="n">
         <f aca="true">RAND()</f>
-        <v>0.907030832900059</v>
+        <v>0.866036193282962</v>
       </c>
       <c r="G61" s="0" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="62" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A62" s="5" t="s">
-        <v>7</v>
-      </c>
-      <c r="B62" s="5" t="s">
-        <v>6</v>
-      </c>
-      <c r="C62" s="6" t="s">
+      <c r="A62" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B62" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C62" s="5" t="s">
         <v>8</v>
       </c>
       <c r="D62" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="E62" s="5"/>
-      <c r="F62" s="5"/>
-      <c r="G62" s="6"/>
+      <c r="E62" s="2"/>
+      <c r="F62" s="2"/>
+      <c r="G62" s="5"/>
     </row>
     <row r="63" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A63" s="5" t="s">
-        <v>7</v>
-      </c>
-      <c r="B63" s="5" t="s">
-        <v>6</v>
-      </c>
-      <c r="C63" s="6" t="s">
+      <c r="A63" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B63" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C63" s="5" t="s">
         <v>8</v>
       </c>
       <c r="D63" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="E63" s="5"/>
-      <c r="F63" s="5"/>
-      <c r="G63" s="6"/>
+      <c r="E63" s="2"/>
+      <c r="F63" s="2"/>
+      <c r="G63" s="5"/>
     </row>
     <row r="64" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A64" s="5" t="s">
-        <v>7</v>
-      </c>
-      <c r="B64" s="5" t="s">
-        <v>6</v>
-      </c>
-      <c r="C64" s="6" t="s">
+      <c r="A64" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B64" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C64" s="5" t="s">
         <v>8</v>
       </c>
       <c r="D64" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="E64" s="5"/>
-      <c r="F64" s="5"/>
-      <c r="G64" s="6"/>
+      <c r="E64" s="2"/>
+      <c r="F64" s="2"/>
+      <c r="G64" s="5"/>
     </row>
     <row r="65" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A65" s="5" t="s">
-        <v>7</v>
-      </c>
-      <c r="B65" s="5" t="s">
-        <v>6</v>
-      </c>
-      <c r="C65" s="6" t="s">
+      <c r="A65" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B65" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C65" s="5" t="s">
         <v>8</v>
       </c>
       <c r="D65" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="E65" s="5"/>
-      <c r="F65" s="5"/>
-      <c r="G65" s="6"/>
+      <c r="E65" s="2"/>
+      <c r="F65" s="2"/>
+      <c r="G65" s="5"/>
     </row>
     <row r="66" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A66" s="5" t="s">
-        <v>7</v>
-      </c>
-      <c r="B66" s="5" t="s">
-        <v>6</v>
-      </c>
-      <c r="C66" s="6" t="s">
+      <c r="A66" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B66" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C66" s="5" t="s">
         <v>12</v>
       </c>
       <c r="D66" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="E66" s="5"/>
-      <c r="F66" s="5"/>
-      <c r="G66" s="6"/>
+      <c r="E66" s="2"/>
+      <c r="F66" s="2"/>
+      <c r="G66" s="5"/>
     </row>
     <row r="67" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A67" s="2" t="s">
@@ -1806,433 +1806,433 @@
       <c r="B67" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="C67" s="6" t="s">
+      <c r="C67" s="5" t="s">
         <v>8</v>
       </c>
       <c r="D67" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="E67" s="5"/>
-      <c r="F67" s="5"/>
-      <c r="G67" s="6"/>
+      <c r="E67" s="2"/>
+      <c r="F67" s="2"/>
+      <c r="G67" s="5"/>
     </row>
     <row r="68" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A68" s="5" t="s">
-        <v>6</v>
-      </c>
-      <c r="B68" s="5" t="s">
-        <v>7</v>
-      </c>
-      <c r="C68" s="6" t="s">
+      <c r="A68" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B68" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C68" s="5" t="s">
         <v>12</v>
       </c>
       <c r="D68" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="E68" s="5"/>
-      <c r="F68" s="5"/>
-      <c r="G68" s="6"/>
+      <c r="E68" s="2"/>
+      <c r="F68" s="2"/>
+      <c r="G68" s="5"/>
     </row>
     <row r="69" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A69" s="5" t="s">
-        <v>6</v>
-      </c>
-      <c r="B69" s="5" t="s">
-        <v>7</v>
-      </c>
-      <c r="C69" s="6" t="s">
+      <c r="A69" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B69" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C69" s="5" t="s">
         <v>8</v>
       </c>
       <c r="D69" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="E69" s="5"/>
-      <c r="F69" s="5"/>
-      <c r="G69" s="6"/>
+      <c r="E69" s="2"/>
+      <c r="F69" s="2"/>
+      <c r="G69" s="5"/>
     </row>
     <row r="70" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A70" s="5" t="s">
-        <v>6</v>
-      </c>
-      <c r="B70" s="5" t="s">
-        <v>7</v>
-      </c>
-      <c r="C70" s="6" t="s">
+      <c r="A70" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B70" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C70" s="5" t="s">
         <v>12</v>
       </c>
       <c r="D70" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="E70" s="5"/>
-      <c r="F70" s="5"/>
-      <c r="G70" s="6"/>
+      <c r="E70" s="2"/>
+      <c r="F70" s="2"/>
+      <c r="G70" s="5"/>
     </row>
     <row r="71" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A71" s="5" t="s">
-        <v>7</v>
-      </c>
-      <c r="B71" s="5" t="s">
-        <v>6</v>
-      </c>
-      <c r="C71" s="6" t="s">
+      <c r="A71" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B71" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C71" s="5" t="s">
         <v>12</v>
       </c>
       <c r="D71" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="E71" s="5"/>
-      <c r="F71" s="5"/>
-      <c r="G71" s="6"/>
+      <c r="E71" s="2"/>
+      <c r="F71" s="2"/>
+      <c r="G71" s="5"/>
     </row>
     <row r="72" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A72" s="5" t="s">
-        <v>6</v>
-      </c>
-      <c r="B72" s="5" t="s">
-        <v>7</v>
-      </c>
-      <c r="C72" s="6" t="s">
+      <c r="A72" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B72" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C72" s="5" t="s">
         <v>12</v>
       </c>
       <c r="D72" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="E72" s="5"/>
-      <c r="F72" s="5"/>
-      <c r="G72" s="6"/>
+      <c r="E72" s="2"/>
+      <c r="F72" s="2"/>
+      <c r="G72" s="5"/>
     </row>
     <row r="73" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A73" s="5"/>
-      <c r="B73" s="5"/>
-      <c r="C73" s="6"/>
+      <c r="A73" s="2"/>
+      <c r="B73" s="2"/>
+      <c r="C73" s="5"/>
       <c r="D73" s="1"/>
-      <c r="E73" s="5"/>
-      <c r="F73" s="5"/>
-      <c r="G73" s="6"/>
+      <c r="E73" s="2"/>
+      <c r="F73" s="2"/>
+      <c r="G73" s="5"/>
     </row>
     <row r="74" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A74" s="5"/>
-      <c r="B74" s="5"/>
-      <c r="C74" s="6"/>
+      <c r="A74" s="2"/>
+      <c r="B74" s="2"/>
+      <c r="C74" s="5"/>
       <c r="D74" s="1"/>
-      <c r="E74" s="5"/>
-      <c r="F74" s="5"/>
-      <c r="G74" s="6"/>
+      <c r="E74" s="2"/>
+      <c r="F74" s="2"/>
+      <c r="G74" s="5"/>
     </row>
     <row r="75" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A75" s="5"/>
-      <c r="B75" s="5"/>
-      <c r="C75" s="6"/>
+      <c r="A75" s="2"/>
+      <c r="B75" s="2"/>
+      <c r="C75" s="5"/>
       <c r="D75" s="1"/>
-      <c r="E75" s="5"/>
-      <c r="F75" s="5"/>
-      <c r="G75" s="6"/>
+      <c r="E75" s="2"/>
+      <c r="F75" s="2"/>
+      <c r="G75" s="5"/>
     </row>
     <row r="76" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A76" s="5"/>
-      <c r="B76" s="5"/>
-      <c r="C76" s="6"/>
+      <c r="A76" s="2"/>
+      <c r="B76" s="2"/>
+      <c r="C76" s="5"/>
       <c r="D76" s="1"/>
-      <c r="E76" s="5"/>
-      <c r="F76" s="5"/>
-      <c r="G76" s="6"/>
+      <c r="E76" s="2"/>
+      <c r="F76" s="2"/>
+      <c r="G76" s="5"/>
     </row>
     <row r="77" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A77" s="5"/>
-      <c r="B77" s="5"/>
-      <c r="C77" s="6"/>
+      <c r="A77" s="2"/>
+      <c r="B77" s="2"/>
+      <c r="C77" s="5"/>
       <c r="D77" s="1"/>
-      <c r="E77" s="5"/>
-      <c r="F77" s="5"/>
-      <c r="G77" s="6"/>
+      <c r="E77" s="2"/>
+      <c r="F77" s="2"/>
+      <c r="G77" s="5"/>
     </row>
     <row r="78" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A78" s="5"/>
-      <c r="B78" s="5"/>
-      <c r="C78" s="6"/>
+      <c r="A78" s="2"/>
+      <c r="B78" s="2"/>
+      <c r="C78" s="5"/>
       <c r="D78" s="1"/>
-      <c r="E78" s="5"/>
-      <c r="F78" s="5"/>
-      <c r="G78" s="6"/>
+      <c r="E78" s="2"/>
+      <c r="F78" s="2"/>
+      <c r="G78" s="5"/>
     </row>
     <row r="79" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A79" s="5"/>
-      <c r="B79" s="5"/>
-      <c r="C79" s="6"/>
+      <c r="A79" s="2"/>
+      <c r="B79" s="2"/>
+      <c r="C79" s="5"/>
       <c r="D79" s="1"/>
-      <c r="E79" s="5"/>
-      <c r="F79" s="5"/>
-      <c r="G79" s="6"/>
+      <c r="E79" s="2"/>
+      <c r="F79" s="2"/>
+      <c r="G79" s="5"/>
     </row>
     <row r="80" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A80" s="5"/>
-      <c r="B80" s="5"/>
-      <c r="C80" s="6"/>
+      <c r="A80" s="2"/>
+      <c r="B80" s="2"/>
+      <c r="C80" s="5"/>
       <c r="D80" s="1"/>
-      <c r="E80" s="5"/>
-      <c r="F80" s="5"/>
-      <c r="G80" s="6"/>
+      <c r="E80" s="2"/>
+      <c r="F80" s="2"/>
+      <c r="G80" s="5"/>
     </row>
     <row r="81" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A81" s="5"/>
-      <c r="B81" s="5"/>
-      <c r="C81" s="6"/>
+      <c r="A81" s="2"/>
+      <c r="B81" s="2"/>
+      <c r="C81" s="5"/>
       <c r="D81" s="1"/>
-      <c r="E81" s="5"/>
-      <c r="F81" s="5"/>
-      <c r="G81" s="6"/>
+      <c r="E81" s="2"/>
+      <c r="F81" s="2"/>
+      <c r="G81" s="5"/>
     </row>
     <row r="82" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A82" s="5"/>
-      <c r="B82" s="5"/>
-      <c r="C82" s="6"/>
+      <c r="A82" s="2"/>
+      <c r="B82" s="2"/>
+      <c r="C82" s="5"/>
       <c r="D82" s="1"/>
-      <c r="E82" s="5"/>
-      <c r="F82" s="5"/>
-      <c r="G82" s="6"/>
+      <c r="E82" s="2"/>
+      <c r="F82" s="2"/>
+      <c r="G82" s="5"/>
     </row>
     <row r="83" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A83" s="5"/>
-      <c r="B83" s="5"/>
-      <c r="C83" s="6"/>
+      <c r="A83" s="2"/>
+      <c r="B83" s="2"/>
+      <c r="C83" s="5"/>
       <c r="D83" s="1"/>
-      <c r="E83" s="5"/>
-      <c r="F83" s="5"/>
-      <c r="G83" s="6"/>
+      <c r="E83" s="2"/>
+      <c r="F83" s="2"/>
+      <c r="G83" s="5"/>
     </row>
     <row r="84" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A84" s="5"/>
-      <c r="B84" s="5"/>
-      <c r="C84" s="6"/>
+      <c r="A84" s="2"/>
+      <c r="B84" s="2"/>
+      <c r="C84" s="5"/>
       <c r="D84" s="1"/>
-      <c r="E84" s="5"/>
-      <c r="F84" s="5"/>
-      <c r="G84" s="6"/>
+      <c r="E84" s="2"/>
+      <c r="F84" s="2"/>
+      <c r="G84" s="5"/>
     </row>
     <row r="85" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A85" s="5"/>
-      <c r="B85" s="5"/>
-      <c r="C85" s="6"/>
+      <c r="A85" s="2"/>
+      <c r="B85" s="2"/>
+      <c r="C85" s="5"/>
       <c r="D85" s="1"/>
-      <c r="E85" s="5"/>
-      <c r="F85" s="5"/>
-      <c r="G85" s="6"/>
+      <c r="E85" s="2"/>
+      <c r="F85" s="2"/>
+      <c r="G85" s="5"/>
     </row>
     <row r="86" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A86" s="5"/>
-      <c r="B86" s="5"/>
-      <c r="C86" s="6"/>
+      <c r="A86" s="2"/>
+      <c r="B86" s="2"/>
+      <c r="C86" s="5"/>
       <c r="D86" s="1"/>
-      <c r="E86" s="5"/>
-      <c r="F86" s="5"/>
-      <c r="G86" s="6"/>
+      <c r="E86" s="2"/>
+      <c r="F86" s="2"/>
+      <c r="G86" s="5"/>
     </row>
     <row r="87" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A87" s="5"/>
-      <c r="B87" s="5"/>
-      <c r="C87" s="6"/>
+      <c r="A87" s="2"/>
+      <c r="B87" s="2"/>
+      <c r="C87" s="5"/>
       <c r="D87" s="1"/>
-      <c r="E87" s="5"/>
-      <c r="F87" s="5"/>
-      <c r="G87" s="6"/>
+      <c r="E87" s="2"/>
+      <c r="F87" s="2"/>
+      <c r="G87" s="5"/>
     </row>
     <row r="88" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A88" s="5"/>
-      <c r="B88" s="5"/>
-      <c r="C88" s="6"/>
+      <c r="A88" s="2"/>
+      <c r="B88" s="2"/>
+      <c r="C88" s="5"/>
       <c r="D88" s="1"/>
-      <c r="E88" s="5"/>
-      <c r="F88" s="5"/>
-      <c r="G88" s="6"/>
+      <c r="E88" s="2"/>
+      <c r="F88" s="2"/>
+      <c r="G88" s="5"/>
     </row>
     <row r="89" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A89" s="5"/>
-      <c r="B89" s="5"/>
-      <c r="C89" s="6"/>
+      <c r="A89" s="2"/>
+      <c r="B89" s="2"/>
+      <c r="C89" s="5"/>
       <c r="D89" s="1"/>
-      <c r="E89" s="5"/>
-      <c r="F89" s="5"/>
-      <c r="G89" s="6"/>
+      <c r="E89" s="2"/>
+      <c r="F89" s="2"/>
+      <c r="G89" s="5"/>
     </row>
     <row r="90" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A90" s="5"/>
-      <c r="B90" s="5"/>
-      <c r="C90" s="6"/>
+      <c r="A90" s="2"/>
+      <c r="B90" s="2"/>
+      <c r="C90" s="5"/>
       <c r="D90" s="1"/>
-      <c r="E90" s="5"/>
-      <c r="F90" s="5"/>
-      <c r="G90" s="6"/>
+      <c r="E90" s="2"/>
+      <c r="F90" s="2"/>
+      <c r="G90" s="5"/>
     </row>
     <row r="91" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A91" s="5"/>
-      <c r="B91" s="5"/>
-      <c r="C91" s="6"/>
+      <c r="A91" s="2"/>
+      <c r="B91" s="2"/>
+      <c r="C91" s="5"/>
       <c r="D91" s="1"/>
-      <c r="E91" s="5"/>
-      <c r="F91" s="5"/>
-      <c r="G91" s="6"/>
+      <c r="E91" s="2"/>
+      <c r="F91" s="2"/>
+      <c r="G91" s="5"/>
     </row>
     <row r="92" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A92" s="5"/>
-      <c r="B92" s="5"/>
-      <c r="C92" s="6"/>
+      <c r="A92" s="2"/>
+      <c r="B92" s="2"/>
+      <c r="C92" s="5"/>
       <c r="D92" s="1"/>
-      <c r="E92" s="5"/>
-      <c r="F92" s="5"/>
-      <c r="G92" s="6"/>
+      <c r="E92" s="2"/>
+      <c r="F92" s="2"/>
+      <c r="G92" s="5"/>
     </row>
     <row r="93" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A93" s="5"/>
-      <c r="B93" s="5"/>
-      <c r="C93" s="6"/>
+      <c r="A93" s="2"/>
+      <c r="B93" s="2"/>
+      <c r="C93" s="5"/>
       <c r="D93" s="1"/>
-      <c r="E93" s="5"/>
-      <c r="F93" s="5"/>
-      <c r="G93" s="6"/>
+      <c r="E93" s="2"/>
+      <c r="F93" s="2"/>
+      <c r="G93" s="5"/>
     </row>
     <row r="94" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A94" s="5"/>
-      <c r="B94" s="5"/>
-      <c r="C94" s="6"/>
+      <c r="A94" s="2"/>
+      <c r="B94" s="2"/>
+      <c r="C94" s="5"/>
       <c r="D94" s="1"/>
-      <c r="E94" s="5"/>
-      <c r="F94" s="5"/>
-      <c r="G94" s="6"/>
+      <c r="E94" s="2"/>
+      <c r="F94" s="2"/>
+      <c r="G94" s="5"/>
     </row>
     <row r="95" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A95" s="5"/>
-      <c r="B95" s="5"/>
-      <c r="C95" s="6"/>
+      <c r="A95" s="2"/>
+      <c r="B95" s="2"/>
+      <c r="C95" s="5"/>
       <c r="D95" s="1"/>
-      <c r="E95" s="5"/>
-      <c r="F95" s="5"/>
-      <c r="G95" s="6"/>
+      <c r="E95" s="2"/>
+      <c r="F95" s="2"/>
+      <c r="G95" s="5"/>
     </row>
     <row r="96" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A96" s="5"/>
-      <c r="B96" s="5"/>
-      <c r="C96" s="6"/>
+      <c r="A96" s="2"/>
+      <c r="B96" s="2"/>
+      <c r="C96" s="5"/>
       <c r="D96" s="1"/>
-      <c r="E96" s="5"/>
-      <c r="F96" s="5"/>
-      <c r="G96" s="6"/>
+      <c r="E96" s="2"/>
+      <c r="F96" s="2"/>
+      <c r="G96" s="5"/>
     </row>
     <row r="97" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A97" s="5"/>
-      <c r="B97" s="5"/>
-      <c r="C97" s="6"/>
+      <c r="A97" s="2"/>
+      <c r="B97" s="2"/>
+      <c r="C97" s="5"/>
       <c r="D97" s="1"/>
-      <c r="E97" s="5"/>
-      <c r="F97" s="5"/>
-      <c r="G97" s="6"/>
+      <c r="E97" s="2"/>
+      <c r="F97" s="2"/>
+      <c r="G97" s="5"/>
     </row>
     <row r="98" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A98" s="5"/>
-      <c r="B98" s="5"/>
-      <c r="C98" s="6"/>
+      <c r="A98" s="2"/>
+      <c r="B98" s="2"/>
+      <c r="C98" s="5"/>
       <c r="D98" s="1"/>
-      <c r="E98" s="5"/>
-      <c r="F98" s="5"/>
-      <c r="G98" s="6"/>
+      <c r="E98" s="2"/>
+      <c r="F98" s="2"/>
+      <c r="G98" s="5"/>
     </row>
     <row r="99" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A99" s="5"/>
-      <c r="B99" s="5"/>
-      <c r="C99" s="6"/>
+      <c r="A99" s="2"/>
+      <c r="B99" s="2"/>
+      <c r="C99" s="5"/>
       <c r="D99" s="1"/>
-      <c r="E99" s="5"/>
-      <c r="F99" s="5"/>
-      <c r="G99" s="6"/>
+      <c r="E99" s="2"/>
+      <c r="F99" s="2"/>
+      <c r="G99" s="5"/>
     </row>
     <row r="100" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A100" s="5"/>
-      <c r="B100" s="5"/>
-      <c r="C100" s="6"/>
+      <c r="A100" s="2"/>
+      <c r="B100" s="2"/>
+      <c r="C100" s="5"/>
       <c r="D100" s="1"/>
-      <c r="E100" s="5"/>
-      <c r="F100" s="5"/>
-      <c r="G100" s="6"/>
+      <c r="E100" s="2"/>
+      <c r="F100" s="2"/>
+      <c r="G100" s="5"/>
     </row>
     <row r="101" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A101" s="5"/>
-      <c r="B101" s="5"/>
-      <c r="C101" s="6"/>
+      <c r="A101" s="2"/>
+      <c r="B101" s="2"/>
+      <c r="C101" s="5"/>
       <c r="D101" s="1"/>
-      <c r="E101" s="5"/>
-      <c r="F101" s="5"/>
-      <c r="G101" s="6"/>
+      <c r="E101" s="2"/>
+      <c r="F101" s="2"/>
+      <c r="G101" s="5"/>
     </row>
     <row r="102" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A102" s="5"/>
-      <c r="B102" s="5"/>
-      <c r="C102" s="6"/>
+      <c r="A102" s="2"/>
+      <c r="B102" s="2"/>
+      <c r="C102" s="5"/>
       <c r="D102" s="1"/>
-      <c r="E102" s="5"/>
-      <c r="F102" s="5"/>
-      <c r="G102" s="6"/>
+      <c r="E102" s="2"/>
+      <c r="F102" s="2"/>
+      <c r="G102" s="5"/>
     </row>
     <row r="103" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A103" s="5"/>
-      <c r="B103" s="5"/>
-      <c r="C103" s="6"/>
+      <c r="A103" s="2"/>
+      <c r="B103" s="2"/>
+      <c r="C103" s="5"/>
       <c r="D103" s="1"/>
-      <c r="E103" s="5"/>
-      <c r="F103" s="5"/>
-      <c r="G103" s="6"/>
+      <c r="E103" s="2"/>
+      <c r="F103" s="2"/>
+      <c r="G103" s="5"/>
     </row>
     <row r="104" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A104" s="5"/>
-      <c r="B104" s="5"/>
-      <c r="C104" s="6"/>
+      <c r="A104" s="2"/>
+      <c r="B104" s="2"/>
+      <c r="C104" s="5"/>
       <c r="D104" s="1"/>
-      <c r="E104" s="5"/>
-      <c r="F104" s="5"/>
-      <c r="G104" s="6"/>
+      <c r="E104" s="2"/>
+      <c r="F104" s="2"/>
+      <c r="G104" s="5"/>
     </row>
     <row r="105" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A105" s="5"/>
-      <c r="B105" s="5"/>
-      <c r="C105" s="6"/>
+      <c r="A105" s="2"/>
+      <c r="B105" s="2"/>
+      <c r="C105" s="5"/>
       <c r="D105" s="1"/>
-      <c r="E105" s="5"/>
-      <c r="F105" s="5"/>
-      <c r="G105" s="6"/>
+      <c r="E105" s="2"/>
+      <c r="F105" s="2"/>
+      <c r="G105" s="5"/>
     </row>
     <row r="106" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A106" s="5"/>
-      <c r="B106" s="5"/>
-      <c r="C106" s="6"/>
+      <c r="A106" s="2"/>
+      <c r="B106" s="2"/>
+      <c r="C106" s="5"/>
       <c r="D106" s="1"/>
-      <c r="E106" s="5"/>
-      <c r="F106" s="5"/>
-      <c r="G106" s="6"/>
+      <c r="E106" s="2"/>
+      <c r="F106" s="2"/>
+      <c r="G106" s="5"/>
     </row>
     <row r="107" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A107" s="5"/>
-      <c r="B107" s="5"/>
-      <c r="C107" s="6"/>
+      <c r="A107" s="2"/>
+      <c r="B107" s="2"/>
+      <c r="C107" s="5"/>
       <c r="D107" s="1"/>
-      <c r="E107" s="5"/>
-      <c r="F107" s="5"/>
-      <c r="G107" s="6"/>
+      <c r="E107" s="2"/>
+      <c r="F107" s="2"/>
+      <c r="G107" s="5"/>
     </row>
     <row r="108" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A108" s="5"/>
-      <c r="B108" s="5"/>
-      <c r="C108" s="6"/>
+      <c r="A108" s="2"/>
+      <c r="B108" s="2"/>
+      <c r="C108" s="5"/>
       <c r="D108" s="1"/>
-      <c r="E108" s="5"/>
-      <c r="F108" s="5"/>
-      <c r="G108" s="6"/>
+      <c r="E108" s="2"/>
+      <c r="F108" s="2"/>
+      <c r="G108" s="5"/>
     </row>
     <row r="109" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A109" s="5"/>
-      <c r="B109" s="5"/>
-      <c r="C109" s="6"/>
+      <c r="A109" s="2"/>
+      <c r="B109" s="2"/>
+      <c r="C109" s="5"/>
       <c r="D109" s="1"/>
-      <c r="E109" s="5"/>
-      <c r="F109" s="5"/>
-      <c r="G109" s="6"/>
+      <c r="E109" s="2"/>
+      <c r="F109" s="2"/>
+      <c r="G109" s="5"/>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>

</xml_diff>